<commit_message>
added protected templates and expansion under coconut folder structure
</commit_message>
<xml_diff>
--- a/src/templates/IECMaterial_Template.xlsx
+++ b/src/templates/IECMaterial_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devvi\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devvi\Desktop\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{890F4175-FB57-4794-A4AF-68148392A871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA4C66E-493C-4EA6-98F6-94A821F5EF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3285" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,6 +143,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -243,14 +244,14 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,14 +481,14 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="1" customWidth="1"/>
     <col min="4" max="7" width="20" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="34.85546875" style="1" customWidth="1"/>
@@ -501,45 +502,45 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -548,13 +549,13 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
@@ -592,37 +593,37 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="12">
         <v>45030</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>1000</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <v>45031</v>
       </c>
     </row>
@@ -1108,6 +1109,7 @@
       <c r="K43" s="2"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="KcZxmMHKZRHGbwwkiI10FuesyMdxU5seMmhConxWVSid/kczdDYCQnHPLItAhElW6fGk8vWyouICNXRQeMRVEg==" saltValue="VWWMXjMpzZx4ZcX1h0FIDw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="E2:K2"/>

</xml_diff>